<commit_message>
fixing namibia point and update model
</commit_message>
<xml_diff>
--- a/Dataset/events_data/Events_data_full_KADI.xlsx
+++ b/Dataset/events_data/Events_data_full_KADI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katri\Documents\Python_scripts\MDA_project\Modern-Data-Analytics-Backend\Dataset\events_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F73689E-2BB3-492F-9701-8712F48FD006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA205721-FD11-490B-B95C-F254FDD27F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{87935243-AA2B-4B1A-92BC-362D0640AA61}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4085" uniqueCount="763">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4085" uniqueCount="764">
   <si>
     <t>Address</t>
   </si>
@@ -2329,6 +2329,9 @@
   </si>
   <si>
     <t>08-05-2022</t>
+  </si>
+  <si>
+    <t>Boekhandelstraat 2, Leuven</t>
   </si>
 </sst>
 </file>
@@ -2748,8 +2751,8 @@
   <dimension ref="A1:L670"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A580" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C663" sqref="C663"/>
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B674" sqref="B674"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2835,7 +2838,7 @@
         <v>69</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:J9" si="0">SUM(H2:I2)</f>
+        <f t="shared" ref="J2:J8" si="0">SUM(H2:I2)</f>
         <v>76</v>
       </c>
     </row>
@@ -3037,7 +3040,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -3132,7 +3135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -3627,7 +3630,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -3688,7 +3691,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -4052,7 +4055,7 @@
         <v>1</v>
       </c>
       <c r="J41">
-        <f>SUM(H41:I41)</f>
+        <f t="shared" ref="J41:J49" si="1">SUM(H41:I41)</f>
         <v>2</v>
       </c>
     </row>
@@ -4083,11 +4086,11 @@
         <v>15</v>
       </c>
       <c r="J42">
-        <f>SUM(H42:I42)</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -4116,7 +4119,7 @@
         <v>286</v>
       </c>
       <c r="J43">
-        <f>SUM(H43:I43)</f>
+        <f t="shared" si="1"/>
         <v>342</v>
       </c>
     </row>
@@ -4149,11 +4152,11 @@
         <v>305</v>
       </c>
       <c r="J44">
-        <f>SUM(H44:I44)</f>
+        <f t="shared" si="1"/>
         <v>322</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>106</v>
       </c>
@@ -4182,7 +4185,7 @@
         <v>282</v>
       </c>
       <c r="J45">
-        <f>SUM(H45:I45)</f>
+        <f t="shared" si="1"/>
         <v>324</v>
       </c>
     </row>
@@ -4215,7 +4218,7 @@
         <v>61</v>
       </c>
       <c r="J46">
-        <f>SUM(H46:I46)</f>
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
     </row>
@@ -4248,7 +4251,7 @@
         <v>261</v>
       </c>
       <c r="J47">
-        <f>SUM(H47:I47)</f>
+        <f t="shared" si="1"/>
         <v>320</v>
       </c>
     </row>
@@ -4281,7 +4284,7 @@
         <v>1</v>
       </c>
       <c r="J48">
-        <f>SUM(H48:I48)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -4314,7 +4317,7 @@
         <v>115</v>
       </c>
       <c r="J49">
-        <f>SUM(H49:I49)</f>
+        <f t="shared" si="1"/>
         <v>145</v>
       </c>
     </row>
@@ -4347,7 +4350,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>46</v>
       </c>
@@ -4785,7 +4788,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>83</v>
       </c>
@@ -4818,7 +4821,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>48</v>
       </c>
@@ -4883,7 +4886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>48</v>
       </c>
@@ -5313,7 +5316,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>27</v>
       </c>
@@ -5412,7 +5415,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>105</v>
       </c>
@@ -5473,7 +5476,7 @@
         <v>15</v>
       </c>
       <c r="J86">
-        <f>SUM(H86:I86)</f>
+        <f t="shared" ref="J86:J91" si="2">SUM(H86:I86)</f>
         <v>22</v>
       </c>
     </row>
@@ -5506,7 +5509,7 @@
         <v>140</v>
       </c>
       <c r="J87">
-        <f>SUM(H87:I87)</f>
+        <f t="shared" si="2"/>
         <v>160</v>
       </c>
     </row>
@@ -5539,7 +5542,7 @@
         <v>37</v>
       </c>
       <c r="J88">
-        <f>SUM(H88:I88)</f>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
     </row>
@@ -5572,11 +5575,11 @@
         <v>58</v>
       </c>
       <c r="J89">
-        <f>SUM(H89:I89)</f>
+        <f t="shared" si="2"/>
         <v>91</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>82</v>
       </c>
@@ -5605,11 +5608,11 @@
         <v>323</v>
       </c>
       <c r="J90">
-        <f>SUM(H90:I90)</f>
+        <f t="shared" si="2"/>
         <v>368</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>70</v>
       </c>
@@ -5638,11 +5641,11 @@
         <v>46</v>
       </c>
       <c r="J91">
-        <f>SUM(H91:I91)</f>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>54</v>
       </c>
@@ -6348,7 +6351,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>36</v>
       </c>
@@ -6468,7 +6471,7 @@
         <v>61</v>
       </c>
       <c r="J118">
-        <f>SUM(H118:I118)</f>
+        <f t="shared" ref="J118:J123" si="3">SUM(H118:I118)</f>
         <v>77</v>
       </c>
     </row>
@@ -6501,7 +6504,7 @@
         <v>13</v>
       </c>
       <c r="J119">
-        <f>SUM(H119:I119)</f>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
     </row>
@@ -6534,7 +6537,7 @@
         <v>117</v>
       </c>
       <c r="J120">
-        <f>SUM(H120:I120)</f>
+        <f t="shared" si="3"/>
         <v>138</v>
       </c>
     </row>
@@ -6567,11 +6570,11 @@
         <v>126</v>
       </c>
       <c r="J121">
-        <f>SUM(H121:I121)</f>
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>81</v>
       </c>
@@ -6600,11 +6603,11 @@
         <v>542</v>
       </c>
       <c r="J122">
-        <f>SUM(H122:I122)</f>
+        <f t="shared" si="3"/>
         <v>632</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>61</v>
       </c>
@@ -6633,7 +6636,7 @@
         <v>70</v>
       </c>
       <c r="J123">
-        <f>SUM(H123:I123)</f>
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
     </row>
@@ -6968,12 +6971,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>213</v>
       </c>
       <c r="B135" t="s">
-        <v>8</v>
+        <v>763</v>
       </c>
       <c r="C135" s="12" t="s">
         <v>533</v>
@@ -7065,7 +7068,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>18</v>
       </c>
@@ -7193,7 +7196,7 @@
         <v>9</v>
       </c>
       <c r="J141">
-        <f>SUM(H141:I141)</f>
+        <f t="shared" ref="J141:J149" si="4">SUM(H141:I141)</f>
         <v>12</v>
       </c>
     </row>
@@ -7226,7 +7229,7 @@
         <v>98</v>
       </c>
       <c r="J142">
-        <f>SUM(H142:I142)</f>
+        <f t="shared" si="4"/>
         <v>113</v>
       </c>
     </row>
@@ -7259,11 +7262,11 @@
         <v>231</v>
       </c>
       <c r="J143">
-        <f>SUM(H143:I143)</f>
+        <f t="shared" si="4"/>
         <v>231</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>92</v>
       </c>
@@ -7292,7 +7295,7 @@
         <v>1100</v>
       </c>
       <c r="J144">
-        <f>SUM(H144:I144)</f>
+        <f t="shared" si="4"/>
         <v>1348</v>
       </c>
     </row>
@@ -7325,7 +7328,7 @@
         <v>53</v>
       </c>
       <c r="J145">
-        <f>SUM(H145:I145)</f>
+        <f t="shared" si="4"/>
         <v>101</v>
       </c>
     </row>
@@ -7358,7 +7361,7 @@
         <v>1</v>
       </c>
       <c r="J146">
-        <f>SUM(H146:I146)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -7391,7 +7394,7 @@
         <v>6</v>
       </c>
       <c r="J147">
-        <f>SUM(H147:I147)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
     </row>
@@ -7424,12 +7427,12 @@
         <v>6900</v>
       </c>
       <c r="J148">
-        <f>SUM(H148:I148)</f>
+        <f t="shared" si="4"/>
         <v>7868</v>
       </c>
       <c r="K148" s="7"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>60</v>
       </c>
@@ -7458,7 +7461,7 @@
         <v>137</v>
       </c>
       <c r="J149">
-        <f>SUM(H149:I149)</f>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
     </row>
@@ -7698,7 +7701,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>35</v>
       </c>
@@ -7857,7 +7860,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>17</v>
       </c>
@@ -7951,7 +7954,7 @@
         <v>24</v>
       </c>
       <c r="J165">
-        <f>SUM(H165:I165)</f>
+        <f t="shared" ref="J165:J174" si="5">SUM(H165:I165)</f>
         <v>36</v>
       </c>
     </row>
@@ -7984,7 +7987,7 @@
         <v>110</v>
       </c>
       <c r="J166">
-        <f>SUM(H166:I166)</f>
+        <f t="shared" si="5"/>
         <v>147</v>
       </c>
     </row>
@@ -8017,11 +8020,11 @@
         <v>59</v>
       </c>
       <c r="J167">
-        <f>SUM(H167:I167)</f>
+        <f t="shared" si="5"/>
         <v>59</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>104</v>
       </c>
@@ -8050,7 +8053,7 @@
         <v>53</v>
       </c>
       <c r="J168">
-        <f>SUM(H168:I168)</f>
+        <f t="shared" si="5"/>
         <v>87</v>
       </c>
     </row>
@@ -8083,7 +8086,7 @@
         <v>125</v>
       </c>
       <c r="J169">
-        <f>SUM(H169:I169)</f>
+        <f t="shared" si="5"/>
         <v>125</v>
       </c>
     </row>
@@ -8116,7 +8119,7 @@
         <v>53</v>
       </c>
       <c r="J170">
-        <f>SUM(H170:I170)</f>
+        <f t="shared" si="5"/>
         <v>101</v>
       </c>
     </row>
@@ -8149,7 +8152,7 @@
         <v>39</v>
       </c>
       <c r="J171">
-        <f>SUM(H171:I171)</f>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
@@ -8182,11 +8185,11 @@
         <v>8</v>
       </c>
       <c r="J172">
-        <f>SUM(H172:I172)</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>48</v>
       </c>
@@ -8215,7 +8218,7 @@
         <v>14</v>
       </c>
       <c r="J173">
-        <f>SUM(H173:I173)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
     </row>
@@ -8248,7 +8251,7 @@
         <v>3</v>
       </c>
       <c r="J174">
-        <f>SUM(H174:I174)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
@@ -8310,7 +8313,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>45</v>
       </c>
@@ -8735,7 +8738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>16</v>
       </c>
@@ -8830,7 +8833,7 @@
         <v>44</v>
       </c>
       <c r="J193">
-        <f>SUM(H193:I193)</f>
+        <f t="shared" ref="J193:J201" si="6">SUM(H193:I193)</f>
         <v>103</v>
       </c>
     </row>
@@ -8863,7 +8866,7 @@
         <v>50</v>
       </c>
       <c r="J194">
-        <f>SUM(H194:I194)</f>
+        <f t="shared" si="6"/>
         <v>84</v>
       </c>
     </row>
@@ -8896,7 +8899,7 @@
         <v>152</v>
       </c>
       <c r="J195">
-        <f>SUM(H195:I195)</f>
+        <f t="shared" si="6"/>
         <v>152</v>
       </c>
     </row>
@@ -8929,7 +8932,7 @@
         <v>51</v>
       </c>
       <c r="J196">
-        <f>SUM(H196:I196)</f>
+        <f t="shared" si="6"/>
         <v>67</v>
       </c>
     </row>
@@ -8962,7 +8965,7 @@
         <v>53</v>
       </c>
       <c r="J197">
-        <f>SUM(H197:I197)</f>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
     </row>
@@ -8995,7 +8998,7 @@
         <v>15</v>
       </c>
       <c r="J198">
-        <f>SUM(H198:I198)</f>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
     </row>
@@ -9028,11 +9031,11 @@
         <v>35</v>
       </c>
       <c r="J199">
-        <f>SUM(H199:I199)</f>
+        <f t="shared" si="6"/>
         <v>42</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>69</v>
       </c>
@@ -9061,7 +9064,7 @@
         <v>132</v>
       </c>
       <c r="J200">
-        <f>SUM(H200:I200)</f>
+        <f t="shared" si="6"/>
         <v>151</v>
       </c>
     </row>
@@ -9094,7 +9097,7 @@
         <v>5</v>
       </c>
       <c r="J201">
-        <f>SUM(H201:I201)</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
@@ -9156,7 +9159,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>44</v>
       </c>
@@ -9527,11 +9530,11 @@
         <v>1100</v>
       </c>
       <c r="J215">
-        <f>SUM(H215:I215)</f>
+        <f t="shared" ref="J215:J221" si="7">SUM(H215:I215)</f>
         <v>1223</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>26</v>
       </c>
@@ -9560,11 +9563,11 @@
         <v>333</v>
       </c>
       <c r="J216">
-        <f>SUM(H216:I216)</f>
+        <f t="shared" si="7"/>
         <v>471</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>103</v>
       </c>
@@ -9593,7 +9596,7 @@
         <v>158</v>
       </c>
       <c r="J217">
-        <f>SUM(H217:I217)</f>
+        <f t="shared" si="7"/>
         <v>189</v>
       </c>
     </row>
@@ -9626,7 +9629,7 @@
         <v>3</v>
       </c>
       <c r="J218">
-        <f>SUM(H218:I218)</f>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
     </row>
@@ -9659,11 +9662,11 @@
         <v>53</v>
       </c>
       <c r="J219">
-        <f>SUM(H219:I219)</f>
+        <f t="shared" si="7"/>
         <v>101</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>80</v>
       </c>
@@ -9692,7 +9695,7 @@
         <v>112</v>
       </c>
       <c r="J220">
-        <f>SUM(H220:I220)</f>
+        <f t="shared" si="7"/>
         <v>128</v>
       </c>
     </row>
@@ -9725,11 +9728,11 @@
         <v>3</v>
       </c>
       <c r="J221">
-        <f>SUM(H221:I221)</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>48</v>
       </c>
@@ -10358,7 +10361,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>53</v>
       </c>
@@ -10912,7 +10915,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>25</v>
       </c>
@@ -11039,7 +11042,7 @@
         <v>15</v>
       </c>
       <c r="J263">
-        <f>SUM(H263:I263)</f>
+        <f t="shared" ref="J263:J269" si="8">SUM(H263:I263)</f>
         <v>24</v>
       </c>
     </row>
@@ -11072,7 +11075,7 @@
         <v>393</v>
       </c>
       <c r="J264">
-        <f>SUM(H264:I264)</f>
+        <f t="shared" si="8"/>
         <v>459</v>
       </c>
     </row>
@@ -11105,7 +11108,7 @@
         <v>25</v>
       </c>
       <c r="J265">
-        <f>SUM(H265:I265)</f>
+        <f t="shared" si="8"/>
         <v>35</v>
       </c>
     </row>
@@ -11138,7 +11141,7 @@
         <v>7</v>
       </c>
       <c r="J266">
-        <f>SUM(H266:I266)</f>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
     </row>
@@ -11171,12 +11174,12 @@
         <v>940</v>
       </c>
       <c r="J267">
-        <f>SUM(H267:I267)</f>
+        <f t="shared" si="8"/>
         <v>1113</v>
       </c>
       <c r="K267" s="7"/>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>52</v>
       </c>
@@ -11205,7 +11208,7 @@
         <v>365</v>
       </c>
       <c r="J268">
-        <f>SUM(H268:I268)</f>
+        <f t="shared" si="8"/>
         <v>452</v>
       </c>
     </row>
@@ -11238,7 +11241,7 @@
         <v>89</v>
       </c>
       <c r="J269">
-        <f>SUM(H269:I269)</f>
+        <f t="shared" si="8"/>
         <v>134</v>
       </c>
     </row>
@@ -11482,7 +11485,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>34</v>
       </c>
@@ -11708,7 +11711,7 @@
         <v>11</v>
       </c>
       <c r="J284">
-        <f>SUM(H284:I284)</f>
+        <f t="shared" ref="J284:J292" si="9">SUM(H284:I284)</f>
         <v>15</v>
       </c>
     </row>
@@ -11741,7 +11744,7 @@
         <v>5</v>
       </c>
       <c r="J285">
-        <f>SUM(H285:I285)</f>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
     </row>
@@ -11774,7 +11777,7 @@
         <v>123</v>
       </c>
       <c r="J286">
-        <f>SUM(H286:I286)</f>
+        <f t="shared" si="9"/>
         <v>123</v>
       </c>
     </row>
@@ -11807,7 +11810,7 @@
         <v>27</v>
       </c>
       <c r="J287">
-        <f>SUM(H287:I287)</f>
+        <f t="shared" si="9"/>
         <v>39</v>
       </c>
     </row>
@@ -11840,11 +11843,11 @@
         <v>8</v>
       </c>
       <c r="J288">
-        <f>SUM(H288:I288)</f>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>48</v>
       </c>
@@ -11873,11 +11876,11 @@
         <v>130</v>
       </c>
       <c r="J289">
-        <f>SUM(H289:I289)</f>
+        <f t="shared" si="9"/>
         <v>155</v>
       </c>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>79</v>
       </c>
@@ -11906,11 +11909,11 @@
         <v>183</v>
       </c>
       <c r="J290">
-        <f>SUM(H290:I290)</f>
+        <f t="shared" si="9"/>
         <v>240</v>
       </c>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>51</v>
       </c>
@@ -11939,7 +11942,7 @@
         <v>93</v>
       </c>
       <c r="J291">
-        <f>SUM(H291:I291)</f>
+        <f t="shared" si="9"/>
         <v>113</v>
       </c>
     </row>
@@ -11972,7 +11975,7 @@
         <v>89</v>
       </c>
       <c r="J292">
-        <f>SUM(H292:I292)</f>
+        <f t="shared" si="9"/>
         <v>134</v>
       </c>
     </row>
@@ -12184,7 +12187,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>33</v>
       </c>
@@ -12508,11 +12511,11 @@
         <v>36</v>
       </c>
       <c r="J309">
-        <f>SUM(H309:I309)</f>
+        <f t="shared" ref="J309:J314" si="10">SUM(H309:I309)</f>
         <v>43</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>91</v>
       </c>
@@ -12541,7 +12544,7 @@
         <v>496</v>
       </c>
       <c r="J310">
-        <f>SUM(H310:I310)</f>
+        <f t="shared" si="10"/>
         <v>583</v>
       </c>
     </row>
@@ -12574,7 +12577,7 @@
         <v>5</v>
       </c>
       <c r="J311">
-        <f>SUM(H311:I311)</f>
+        <f t="shared" si="10"/>
         <v>9</v>
       </c>
     </row>
@@ -12607,12 +12610,12 @@
         <v>6900</v>
       </c>
       <c r="J312">
-        <f>SUM(H312:I312)</f>
+        <f t="shared" si="10"/>
         <v>7765</v>
       </c>
       <c r="K312" s="7"/>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>59</v>
       </c>
@@ -12641,7 +12644,7 @@
         <v>109</v>
       </c>
       <c r="J313">
-        <f>SUM(H313:I313)</f>
+        <f t="shared" si="10"/>
         <v>128</v>
       </c>
     </row>
@@ -12674,7 +12677,7 @@
         <v>89</v>
       </c>
       <c r="J314">
-        <f>SUM(H314:I314)</f>
+        <f t="shared" si="10"/>
         <v>134</v>
       </c>
     </row>
@@ -12856,7 +12859,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>32</v>
       </c>
@@ -13082,7 +13085,7 @@
         <v>154</v>
       </c>
       <c r="J327">
-        <f>SUM(H327:I327)</f>
+        <f t="shared" ref="J327:J338" si="11">SUM(H327:I327)</f>
         <v>169</v>
       </c>
     </row>
@@ -13115,7 +13118,7 @@
         <v>90</v>
       </c>
       <c r="J328">
-        <f>SUM(H328:I328)</f>
+        <f t="shared" si="11"/>
         <v>125</v>
       </c>
     </row>
@@ -13148,7 +13151,7 @@
         <v>239</v>
       </c>
       <c r="J329">
-        <f>SUM(H329:I329)</f>
+        <f t="shared" si="11"/>
         <v>390</v>
       </c>
     </row>
@@ -13181,7 +13184,7 @@
         <v>14</v>
       </c>
       <c r="J330">
-        <f>SUM(H330:I330)</f>
+        <f t="shared" si="11"/>
         <v>26</v>
       </c>
     </row>
@@ -13214,11 +13217,11 @@
         <v>253</v>
       </c>
       <c r="J331">
-        <f>SUM(H331:I331)</f>
+        <f t="shared" si="11"/>
         <v>428</v>
       </c>
     </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>102</v>
       </c>
@@ -13247,11 +13250,11 @@
         <v>653</v>
       </c>
       <c r="J332">
-        <f>SUM(H332:I332)</f>
+        <f t="shared" si="11"/>
         <v>747</v>
       </c>
     </row>
-    <row r="333" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>90</v>
       </c>
@@ -13280,7 +13283,7 @@
         <v>58</v>
       </c>
       <c r="J333">
-        <f>SUM(H333:I333)</f>
+        <f t="shared" si="11"/>
         <v>83</v>
       </c>
     </row>
@@ -13313,7 +13316,7 @@
         <v>25</v>
       </c>
       <c r="J334">
-        <f>SUM(H334:I334)</f>
+        <f t="shared" si="11"/>
         <v>31</v>
       </c>
     </row>
@@ -13346,7 +13349,7 @@
         <v>27</v>
       </c>
       <c r="J335">
-        <f>SUM(H335:I335)</f>
+        <f t="shared" si="11"/>
         <v>30</v>
       </c>
     </row>
@@ -13379,11 +13382,11 @@
         <v>1</v>
       </c>
       <c r="J336">
-        <f>SUM(H336:I336)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>48</v>
       </c>
@@ -13412,7 +13415,7 @@
         <v>18</v>
       </c>
       <c r="J337">
-        <f>SUM(H337:I337)</f>
+        <f t="shared" si="11"/>
         <v>21</v>
       </c>
     </row>
@@ -13445,7 +13448,7 @@
         <v>0</v>
       </c>
       <c r="J338">
-        <f>SUM(H338:I338)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -13507,7 +13510,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>43</v>
       </c>
@@ -13821,7 +13824,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>24</v>
       </c>
@@ -13916,7 +13919,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="354" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>15</v>
       </c>
@@ -14010,7 +14013,7 @@
         <v>572</v>
       </c>
       <c r="J356">
-        <f>SUM(H356:I356)</f>
+        <f t="shared" ref="J356:J365" si="12">SUM(H356:I356)</f>
         <v>641</v>
       </c>
     </row>
@@ -14043,7 +14046,7 @@
         <v>15</v>
       </c>
       <c r="J357">
-        <f>SUM(H357:I357)</f>
+        <f t="shared" si="12"/>
         <v>24</v>
       </c>
     </row>
@@ -14076,7 +14079,7 @@
         <v>51</v>
       </c>
       <c r="J358">
-        <f>SUM(H358:I358)</f>
+        <f t="shared" si="12"/>
         <v>51</v>
       </c>
     </row>
@@ -14109,7 +14112,7 @@
         <v>253</v>
       </c>
       <c r="J359">
-        <f>SUM(H359:I359)</f>
+        <f t="shared" si="12"/>
         <v>428</v>
       </c>
     </row>
@@ -14142,11 +14145,11 @@
         <v>11</v>
       </c>
       <c r="J360">
-        <f>SUM(H360:I360)</f>
+        <f t="shared" si="12"/>
         <v>18</v>
       </c>
     </row>
-    <row r="361" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>101</v>
       </c>
@@ -14175,11 +14178,11 @@
         <v>26</v>
       </c>
       <c r="J361">
-        <f>SUM(H361:I361)</f>
+        <f t="shared" si="12"/>
         <v>43</v>
       </c>
     </row>
-    <row r="362" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>100</v>
       </c>
@@ -14208,11 +14211,11 @@
         <v>153</v>
       </c>
       <c r="J362">
-        <f>SUM(H362:I362)</f>
+        <f t="shared" si="12"/>
         <v>188</v>
       </c>
     </row>
-    <row r="363" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>89</v>
       </c>
@@ -14241,7 +14244,7 @@
         <v>152</v>
       </c>
       <c r="J363">
-        <f>SUM(H363:I363)</f>
+        <f t="shared" si="12"/>
         <v>197</v>
       </c>
     </row>
@@ -14274,11 +14277,11 @@
         <v>45</v>
       </c>
       <c r="J364">
-        <f>SUM(H364:I364)</f>
+        <f t="shared" si="12"/>
         <v>49</v>
       </c>
     </row>
-    <row r="365" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>78</v>
       </c>
@@ -14307,11 +14310,11 @@
         <v>94</v>
       </c>
       <c r="J365">
-        <f>SUM(H365:I365)</f>
+        <f t="shared" si="12"/>
         <v>139</v>
       </c>
     </row>
-    <row r="366" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>48</v>
       </c>
@@ -14434,7 +14437,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="370" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>42</v>
       </c>
@@ -14914,7 +14917,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="386" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
         <v>14</v>
       </c>
@@ -14980,7 +14983,7 @@
       </c>
       <c r="K387" s="7"/>
     </row>
-    <row r="388" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
         <v>111</v>
       </c>
@@ -15009,11 +15012,11 @@
         <v>324</v>
       </c>
       <c r="J388">
-        <f>SUM(H388:I388)</f>
+        <f t="shared" ref="J388:J393" si="13">SUM(H388:I388)</f>
         <v>437</v>
       </c>
     </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>99</v>
       </c>
@@ -15042,7 +15045,7 @@
         <v>53</v>
       </c>
       <c r="J389">
-        <f>SUM(H389:I389)</f>
+        <f t="shared" si="13"/>
         <v>65</v>
       </c>
     </row>
@@ -15075,7 +15078,7 @@
         <v>195</v>
       </c>
       <c r="J390">
-        <f>SUM(H390:I390)</f>
+        <f t="shared" si="13"/>
         <v>231</v>
       </c>
     </row>
@@ -15108,11 +15111,11 @@
         <v>253</v>
       </c>
       <c r="J391">
-        <f>SUM(H391:I391)</f>
+        <f t="shared" si="13"/>
         <v>281</v>
       </c>
     </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>68</v>
       </c>
@@ -15141,7 +15144,7 @@
         <v>104</v>
       </c>
       <c r="J392">
-        <f>SUM(H392:I392)</f>
+        <f t="shared" si="13"/>
         <v>127</v>
       </c>
     </row>
@@ -15174,11 +15177,11 @@
         <v>0</v>
       </c>
       <c r="J393">
-        <f>SUM(H393:I393)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>48</v>
       </c>
@@ -15516,7 +15519,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="405" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>23</v>
       </c>
@@ -15611,7 +15614,7 @@
         <v>30</v>
       </c>
       <c r="J407">
-        <f>SUM(H407:I407)</f>
+        <f t="shared" ref="J407:J416" si="14">SUM(H407:I407)</f>
         <v>88</v>
       </c>
     </row>
@@ -15644,7 +15647,7 @@
         <v>32</v>
       </c>
       <c r="J408">
-        <f>SUM(H408:I408)</f>
+        <f t="shared" si="14"/>
         <v>44</v>
       </c>
     </row>
@@ -15677,11 +15680,11 @@
         <v>19</v>
       </c>
       <c r="J409">
-        <f>SUM(H409:I409)</f>
+        <f t="shared" si="14"/>
         <v>29</v>
       </c>
     </row>
-    <row r="410" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>98</v>
       </c>
@@ -15710,7 +15713,7 @@
         <v>269</v>
       </c>
       <c r="J410">
-        <f>SUM(H410:I410)</f>
+        <f t="shared" si="14"/>
         <v>334</v>
       </c>
     </row>
@@ -15743,7 +15746,7 @@
         <v>36</v>
       </c>
       <c r="J411">
-        <f>SUM(H411:I411)</f>
+        <f t="shared" si="14"/>
         <v>51</v>
       </c>
     </row>
@@ -15776,7 +15779,7 @@
         <v>166</v>
       </c>
       <c r="J412">
-        <f>SUM(H412:I412)</f>
+        <f t="shared" si="14"/>
         <v>166</v>
       </c>
     </row>
@@ -15809,7 +15812,7 @@
         <v>44</v>
       </c>
       <c r="J413">
-        <f>SUM(H413:I413)</f>
+        <f t="shared" si="14"/>
         <v>44</v>
       </c>
     </row>
@@ -15842,7 +15845,7 @@
         <v>236</v>
       </c>
       <c r="J414">
-        <f>SUM(H414:I414)</f>
+        <f t="shared" si="14"/>
         <v>263</v>
       </c>
     </row>
@@ -15875,11 +15878,11 @@
         <v>55</v>
       </c>
       <c r="J415">
-        <f>SUM(H415:I415)</f>
+        <f t="shared" si="14"/>
         <v>61</v>
       </c>
     </row>
-    <row r="416" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
         <v>77</v>
       </c>
@@ -15908,7 +15911,7 @@
         <v>539</v>
       </c>
       <c r="J416">
-        <f>SUM(H416:I416)</f>
+        <f t="shared" si="14"/>
         <v>632</v>
       </c>
     </row>
@@ -16189,7 +16192,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="426" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
         <v>22</v>
       </c>
@@ -16255,7 +16258,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="428" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
         <v>88</v>
       </c>
@@ -16288,7 +16291,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="429" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
         <v>76</v>
       </c>
@@ -16321,7 +16324,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="430" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
         <v>58</v>
       </c>
@@ -16353,7 +16356,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="431" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
         <v>50</v>
       </c>
@@ -16762,7 +16765,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="444" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A444" t="s">
         <v>31</v>
       </c>
@@ -16951,7 +16954,7 @@
         <v>196</v>
       </c>
       <c r="J449">
-        <f>SUM(H449:I449)</f>
+        <f t="shared" ref="J449:J457" si="15">SUM(H449:I449)</f>
         <v>295</v>
       </c>
     </row>
@@ -16984,7 +16987,7 @@
         <v>341</v>
       </c>
       <c r="J450">
-        <f>SUM(H450:I450)</f>
+        <f t="shared" si="15"/>
         <v>411</v>
       </c>
     </row>
@@ -17017,7 +17020,7 @@
         <v>339</v>
       </c>
       <c r="J451">
-        <f>SUM(H451:I451)</f>
+        <f t="shared" si="15"/>
         <v>339</v>
       </c>
     </row>
@@ -17050,7 +17053,7 @@
         <v>103</v>
       </c>
       <c r="J452">
-        <f>SUM(H452:I452)</f>
+        <f t="shared" si="15"/>
         <v>122</v>
       </c>
     </row>
@@ -17083,11 +17086,11 @@
         <v>87</v>
       </c>
       <c r="J453">
-        <f>SUM(H453:I453)</f>
+        <f t="shared" si="15"/>
         <v>116</v>
       </c>
     </row>
-    <row r="454" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A454" t="s">
         <v>87</v>
       </c>
@@ -17116,11 +17119,11 @@
         <v>130</v>
       </c>
       <c r="J454">
-        <f>SUM(H454:I454)</f>
+        <f t="shared" si="15"/>
         <v>154</v>
       </c>
     </row>
-    <row r="455" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A455" t="s">
         <v>75</v>
       </c>
@@ -17149,11 +17152,11 @@
         <v>210</v>
       </c>
       <c r="J455">
-        <f>SUM(H455:I455)</f>
+        <f t="shared" si="15"/>
         <v>274</v>
       </c>
     </row>
-    <row r="456" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A456" t="s">
         <v>57</v>
       </c>
@@ -17182,7 +17185,7 @@
         <v>58</v>
       </c>
       <c r="J456">
-        <f>SUM(H456:I456)</f>
+        <f t="shared" si="15"/>
         <v>68</v>
       </c>
     </row>
@@ -17215,7 +17218,7 @@
         <v>16</v>
       </c>
       <c r="J457">
-        <f>SUM(H457:I457)</f>
+        <f t="shared" si="15"/>
         <v>33</v>
       </c>
     </row>
@@ -17310,7 +17313,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="461" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
         <v>41</v>
       </c>
@@ -17492,7 +17495,7 @@
         <v>35</v>
       </c>
       <c r="J466">
-        <f>SUM(H466:I466)</f>
+        <f t="shared" ref="J466:J473" si="16">SUM(H466:I466)</f>
         <v>68</v>
       </c>
     </row>
@@ -17525,7 +17528,7 @@
         <v>64</v>
       </c>
       <c r="J467">
-        <f>SUM(H467:I467)</f>
+        <f t="shared" si="16"/>
         <v>93</v>
       </c>
     </row>
@@ -17558,7 +17561,7 @@
         <v>9</v>
       </c>
       <c r="J468">
-        <f>SUM(H468:I468)</f>
+        <f t="shared" si="16"/>
         <v>14</v>
       </c>
     </row>
@@ -17591,7 +17594,7 @@
         <v>113</v>
       </c>
       <c r="J469">
-        <f>SUM(H469:I469)</f>
+        <f t="shared" si="16"/>
         <v>169</v>
       </c>
     </row>
@@ -17624,7 +17627,7 @@
         <v>18</v>
       </c>
       <c r="J470">
-        <f>SUM(H470:I470)</f>
+        <f t="shared" si="16"/>
         <v>25</v>
       </c>
     </row>
@@ -17657,7 +17660,7 @@
         <v>57</v>
       </c>
       <c r="J471">
-        <f>SUM(H471:I471)</f>
+        <f t="shared" si="16"/>
         <v>76</v>
       </c>
     </row>
@@ -17690,7 +17693,7 @@
         <v>357</v>
       </c>
       <c r="J472">
-        <f>SUM(H472:I472)</f>
+        <f t="shared" si="16"/>
         <v>390</v>
       </c>
     </row>
@@ -17723,11 +17726,11 @@
         <v>6</v>
       </c>
       <c r="J473">
-        <f>SUM(H473:I473)</f>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
     </row>
-    <row r="474" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A474" t="s">
         <v>67</v>
       </c>
@@ -17793,7 +17796,7 @@
       </c>
       <c r="K475" s="7"/>
     </row>
-    <row r="476" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A476" t="s">
         <v>56</v>
       </c>
@@ -17917,7 +17920,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="480" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A480" t="s">
         <v>40</v>
       </c>
@@ -18132,7 +18135,7 @@
         <v>1200</v>
       </c>
       <c r="J486">
-        <f>SUM(H486:I486)</f>
+        <f t="shared" ref="J486:J492" si="17">SUM(H486:I486)</f>
         <v>1283</v>
       </c>
     </row>
@@ -18165,7 +18168,7 @@
         <v>346</v>
       </c>
       <c r="J487">
-        <f>SUM(H487:I487)</f>
+        <f t="shared" si="17"/>
         <v>373</v>
       </c>
     </row>
@@ -18198,7 +18201,7 @@
         <v>53</v>
       </c>
       <c r="J488">
-        <f>SUM(H488:I488)</f>
+        <f t="shared" si="17"/>
         <v>63</v>
       </c>
     </row>
@@ -18231,7 +18234,7 @@
         <v>52</v>
       </c>
       <c r="J489">
-        <f>SUM(H489:I489)</f>
+        <f t="shared" si="17"/>
         <v>79</v>
       </c>
     </row>
@@ -18264,7 +18267,7 @@
         <v>240</v>
       </c>
       <c r="J490">
-        <f>SUM(H490:I490)</f>
+        <f t="shared" si="17"/>
         <v>269</v>
       </c>
     </row>
@@ -18297,11 +18300,11 @@
         <v>19</v>
       </c>
       <c r="J491">
-        <f>SUM(H491:I491)</f>
+        <f t="shared" si="17"/>
         <v>29</v>
       </c>
     </row>
-    <row r="492" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
         <v>110</v>
       </c>
@@ -18330,7 +18333,7 @@
         <v>78</v>
       </c>
       <c r="J492">
-        <f>SUM(H492:I492)</f>
+        <f t="shared" si="17"/>
         <v>102</v>
       </c>
     </row>
@@ -18432,7 +18435,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="496" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
         <v>97</v>
       </c>
@@ -18465,7 +18468,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="497" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>66</v>
       </c>
@@ -18654,7 +18657,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="503" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
         <v>39</v>
       </c>
@@ -18803,7 +18806,7 @@
         <v>448</v>
       </c>
       <c r="J507">
-        <f>SUM(H507:I507)</f>
+        <f t="shared" ref="J507:J523" si="18">SUM(H507:I507)</f>
         <v>612</v>
       </c>
     </row>
@@ -18836,7 +18839,7 @@
         <v>55</v>
       </c>
       <c r="J508">
-        <f>SUM(H508:I508)</f>
+        <f t="shared" si="18"/>
         <v>66</v>
       </c>
     </row>
@@ -18869,7 +18872,7 @@
         <v>19</v>
       </c>
       <c r="J509">
-        <f>SUM(H509:I509)</f>
+        <f t="shared" si="18"/>
         <v>22</v>
       </c>
     </row>
@@ -18902,11 +18905,11 @@
         <v>58</v>
       </c>
       <c r="J510">
-        <f>SUM(H510:I510)</f>
+        <f t="shared" si="18"/>
         <v>69</v>
       </c>
     </row>
-    <row r="511" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
         <v>13</v>
       </c>
@@ -18935,7 +18938,7 @@
         <v>125</v>
       </c>
       <c r="J511">
-        <f>SUM(H511:I511)</f>
+        <f t="shared" si="18"/>
         <v>147</v>
       </c>
     </row>
@@ -18968,7 +18971,7 @@
         <v>57</v>
       </c>
       <c r="J512">
-        <f>SUM(H512:I512)</f>
+        <f t="shared" si="18"/>
         <v>77</v>
       </c>
     </row>
@@ -19001,7 +19004,7 @@
         <v>119</v>
       </c>
       <c r="J513">
-        <f>SUM(H513:I513)</f>
+        <f t="shared" si="18"/>
         <v>128</v>
       </c>
     </row>
@@ -19034,7 +19037,7 @@
         <v>122</v>
       </c>
       <c r="J514">
-        <f>SUM(H514:I514)</f>
+        <f t="shared" si="18"/>
         <v>122</v>
       </c>
     </row>
@@ -19067,11 +19070,11 @@
         <v>1400</v>
       </c>
       <c r="J515">
-        <f>SUM(H515:I515)</f>
+        <f t="shared" si="18"/>
         <v>1673</v>
       </c>
     </row>
-    <row r="516" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A516" t="s">
         <v>109</v>
       </c>
@@ -19100,7 +19103,7 @@
         <v>1000</v>
       </c>
       <c r="J516">
-        <f>SUM(H516:I516)</f>
+        <f t="shared" si="18"/>
         <v>1162</v>
       </c>
     </row>
@@ -19133,7 +19136,7 @@
         <v>42</v>
       </c>
       <c r="J517">
-        <f>SUM(H517:I517)</f>
+        <f t="shared" si="18"/>
         <v>44</v>
       </c>
     </row>
@@ -19166,7 +19169,7 @@
         <v>84</v>
       </c>
       <c r="J518">
-        <f>SUM(H518:I518)</f>
+        <f t="shared" si="18"/>
         <v>97</v>
       </c>
     </row>
@@ -19199,7 +19202,7 @@
         <v>784</v>
       </c>
       <c r="J519">
-        <f>SUM(H519:I519)</f>
+        <f t="shared" si="18"/>
         <v>835</v>
       </c>
     </row>
@@ -19232,7 +19235,7 @@
         <v>103</v>
       </c>
       <c r="J520">
-        <f>SUM(H520:I520)</f>
+        <f t="shared" si="18"/>
         <v>164</v>
       </c>
     </row>
@@ -19265,11 +19268,11 @@
         <v>23</v>
       </c>
       <c r="J521">
-        <f>SUM(H521:I521)</f>
+        <f t="shared" si="18"/>
         <v>28</v>
       </c>
     </row>
-    <row r="522" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A522" t="s">
         <v>65</v>
       </c>
@@ -19298,7 +19301,7 @@
         <v>229</v>
       </c>
       <c r="J522">
-        <f>SUM(H522:I522)</f>
+        <f t="shared" si="18"/>
         <v>265</v>
       </c>
     </row>
@@ -19331,7 +19334,7 @@
         <v>0</v>
       </c>
       <c r="J523">
-        <f>SUM(H523:I523)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -19393,7 +19396,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="526" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A526" t="s">
         <v>38</v>
       </c>
@@ -19550,7 +19553,7 @@
         <v>134</v>
       </c>
       <c r="J530">
-        <f>SUM(H530:I530)</f>
+        <f t="shared" ref="J530:J540" si="19">SUM(H530:I530)</f>
         <v>144</v>
       </c>
     </row>
@@ -19583,7 +19586,7 @@
         <v>102</v>
       </c>
       <c r="J531">
-        <f>SUM(H531:I531)</f>
+        <f t="shared" si="19"/>
         <v>154</v>
       </c>
     </row>
@@ -19616,7 +19619,7 @@
         <v>54</v>
       </c>
       <c r="J532">
-        <f>SUM(H532:I532)</f>
+        <f t="shared" si="19"/>
         <v>59</v>
       </c>
     </row>
@@ -19649,7 +19652,7 @@
         <v>38</v>
       </c>
       <c r="J533">
-        <f>SUM(H533:I533)</f>
+        <f t="shared" si="19"/>
         <v>46</v>
       </c>
     </row>
@@ -19682,11 +19685,11 @@
         <v>3600</v>
       </c>
       <c r="J534">
-        <f>SUM(H534:I534)</f>
+        <f t="shared" si="19"/>
         <v>5900</v>
       </c>
     </row>
-    <row r="535" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="535" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A535" t="s">
         <v>108</v>
       </c>
@@ -19715,7 +19718,7 @@
         <v>310</v>
       </c>
       <c r="J535">
-        <f>SUM(H535:I535)</f>
+        <f t="shared" si="19"/>
         <v>477</v>
       </c>
     </row>
@@ -19748,7 +19751,7 @@
         <v>42</v>
       </c>
       <c r="J536">
-        <f>SUM(H536:I536)</f>
+        <f t="shared" si="19"/>
         <v>57</v>
       </c>
     </row>
@@ -19781,7 +19784,7 @@
         <v>98</v>
       </c>
       <c r="J537">
-        <f>SUM(H537:I537)</f>
+        <f t="shared" si="19"/>
         <v>117</v>
       </c>
     </row>
@@ -19814,11 +19817,11 @@
         <v>27</v>
       </c>
       <c r="J538">
-        <f>SUM(H538:I538)</f>
+        <f t="shared" si="19"/>
         <v>32</v>
       </c>
     </row>
-    <row r="539" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="539" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A539" t="s">
         <v>74</v>
       </c>
@@ -19847,11 +19850,11 @@
         <v>224</v>
       </c>
       <c r="J539">
-        <f>SUM(H539:I539)</f>
+        <f t="shared" si="19"/>
         <v>306</v>
       </c>
     </row>
-    <row r="540" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="540" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A540" t="s">
         <v>64</v>
       </c>
@@ -19880,11 +19883,11 @@
         <v>59</v>
       </c>
       <c r="J540">
-        <f>SUM(H540:I540)</f>
+        <f t="shared" si="19"/>
         <v>70</v>
       </c>
     </row>
-    <row r="541" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="541" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A541" t="s">
         <v>48</v>
       </c>
@@ -20226,7 +20229,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="552" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="552" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A552" t="s">
         <v>107</v>
       </c>
@@ -20259,7 +20262,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="553" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A553" t="s">
         <v>96</v>
       </c>
@@ -20391,7 +20394,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="557" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="557" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A557" t="s">
         <v>73</v>
       </c>
@@ -20783,7 +20786,7 @@
         <v>29</v>
       </c>
       <c r="J569">
-        <f>SUM(H569:I569)</f>
+        <f t="shared" ref="J569:J582" si="20">SUM(H569:I569)</f>
         <v>34</v>
       </c>
     </row>
@@ -20816,11 +20819,11 @@
         <v>2</v>
       </c>
       <c r="J570">
-        <f>SUM(H570:I570)</f>
+        <f t="shared" si="20"/>
         <v>4</v>
       </c>
     </row>
-    <row r="571" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="571" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A571" t="s">
         <v>30</v>
       </c>
@@ -20849,11 +20852,11 @@
         <v>439</v>
       </c>
       <c r="J571">
-        <f>SUM(H571:I571)</f>
+        <f t="shared" si="20"/>
         <v>485</v>
       </c>
     </row>
-    <row r="572" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="572" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A572" t="s">
         <v>21</v>
       </c>
@@ -20882,7 +20885,7 @@
         <v>139</v>
       </c>
       <c r="J572">
-        <f>SUM(H572:I572)</f>
+        <f t="shared" si="20"/>
         <v>171</v>
       </c>
     </row>
@@ -20915,7 +20918,7 @@
         <v>110</v>
       </c>
       <c r="J573">
-        <f>SUM(H573:I573)</f>
+        <f t="shared" si="20"/>
         <v>123</v>
       </c>
     </row>
@@ -20948,7 +20951,7 @@
         <v>30</v>
       </c>
       <c r="J574">
-        <f>SUM(H574:I574)</f>
+        <f t="shared" si="20"/>
         <v>37</v>
       </c>
     </row>
@@ -20981,7 +20984,7 @@
         <v>309</v>
       </c>
       <c r="J575">
-        <f>SUM(H575:I575)</f>
+        <f t="shared" si="20"/>
         <v>423</v>
       </c>
     </row>
@@ -21014,11 +21017,11 @@
         <v>59</v>
       </c>
       <c r="J576">
-        <f>SUM(H576:I576)</f>
+        <f t="shared" si="20"/>
         <v>74</v>
       </c>
     </row>
-    <row r="577" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="577" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A577" t="s">
         <v>72</v>
       </c>
@@ -21047,7 +21050,7 @@
         <v>109</v>
       </c>
       <c r="J577">
-        <f>SUM(H577:I577)</f>
+        <f t="shared" si="20"/>
         <v>130</v>
       </c>
     </row>
@@ -21080,7 +21083,7 @@
         <v>37</v>
       </c>
       <c r="J578">
-        <f>SUM(H578:I578)</f>
+        <f t="shared" si="20"/>
         <v>42</v>
       </c>
     </row>
@@ -21113,11 +21116,11 @@
         <v>4</v>
       </c>
       <c r="J579">
-        <f>SUM(H579:I579)</f>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
     </row>
-    <row r="580" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="580" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A580" t="s">
         <v>49</v>
       </c>
@@ -21146,7 +21149,7 @@
         <v>265</v>
       </c>
       <c r="J580">
-        <f>SUM(H580:I580)</f>
+        <f t="shared" si="20"/>
         <v>321</v>
       </c>
     </row>
@@ -21179,7 +21182,7 @@
         <v>8</v>
       </c>
       <c r="J581">
-        <f>SUM(H581:I581)</f>
+        <f t="shared" si="20"/>
         <v>19</v>
       </c>
     </row>
@@ -21212,7 +21215,7 @@
         <v>37</v>
       </c>
       <c r="J582">
-        <f>SUM(H582:I582)</f>
+        <f t="shared" si="20"/>
         <v>60</v>
       </c>
     </row>
@@ -21514,7 +21517,7 @@
         <v>28</v>
       </c>
       <c r="J592">
-        <f>SUM(H592:I592)</f>
+        <f t="shared" ref="J592:J605" si="21">SUM(H592:I592)</f>
         <v>36</v>
       </c>
     </row>
@@ -21547,7 +21550,7 @@
         <v>0</v>
       </c>
       <c r="J593">
-        <f>SUM(H593:I593)</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
     </row>
@@ -21580,7 +21583,7 @@
         <v>35</v>
       </c>
       <c r="J594">
-        <f>SUM(H594:I594)</f>
+        <f t="shared" si="21"/>
         <v>38</v>
       </c>
     </row>
@@ -21613,7 +21616,7 @@
         <v>367</v>
       </c>
       <c r="J595">
-        <f>SUM(H595:I595)</f>
+        <f t="shared" si="21"/>
         <v>604</v>
       </c>
     </row>
@@ -21646,7 +21649,7 @@
         <v>71</v>
       </c>
       <c r="J596">
-        <f>SUM(H596:I596)</f>
+        <f t="shared" si="21"/>
         <v>108</v>
       </c>
     </row>
@@ -21679,7 +21682,7 @@
         <v>62</v>
       </c>
       <c r="J597">
-        <f>SUM(H597:I597)</f>
+        <f t="shared" si="21"/>
         <v>69</v>
       </c>
     </row>
@@ -21712,7 +21715,7 @@
         <v>27</v>
       </c>
       <c r="J598">
-        <f>SUM(H598:I598)</f>
+        <f t="shared" si="21"/>
         <v>34</v>
       </c>
     </row>
@@ -21745,11 +21748,11 @@
         <v>100</v>
       </c>
       <c r="J599">
-        <f>SUM(H599:I599)</f>
+        <f t="shared" si="21"/>
         <v>152</v>
       </c>
     </row>
-    <row r="600" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="600" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A600" t="s">
         <v>86</v>
       </c>
@@ -21778,11 +21781,11 @@
         <v>1200</v>
       </c>
       <c r="J600">
-        <f>SUM(H600:I600)</f>
+        <f t="shared" si="21"/>
         <v>1294</v>
       </c>
     </row>
-    <row r="601" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="601" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A601" t="s">
         <v>71</v>
       </c>
@@ -21811,7 +21814,7 @@
         <v>368</v>
       </c>
       <c r="J601">
-        <f>SUM(H601:I601)</f>
+        <f t="shared" si="21"/>
         <v>415</v>
       </c>
     </row>
@@ -21844,7 +21847,7 @@
         <v>14</v>
       </c>
       <c r="J602">
-        <f>SUM(H602:I602)</f>
+        <f t="shared" si="21"/>
         <v>17</v>
       </c>
     </row>
@@ -21877,11 +21880,11 @@
         <v>1</v>
       </c>
       <c r="J603">
-        <f>SUM(H603:I603)</f>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
     </row>
-    <row r="604" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="604" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A604" t="s">
         <v>48</v>
       </c>
@@ -21910,7 +21913,7 @@
         <v>15</v>
       </c>
       <c r="J604">
-        <f>SUM(H604:I604)</f>
+        <f t="shared" si="21"/>
         <v>16</v>
       </c>
     </row>
@@ -21943,7 +21946,7 @@
         <v>8</v>
       </c>
       <c r="J605">
-        <f>SUM(H605:I605)</f>
+        <f t="shared" si="21"/>
         <v>21</v>
       </c>
     </row>
@@ -22220,7 +22223,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="615" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="615" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A615" t="s">
         <v>29</v>
       </c>
@@ -22509,7 +22512,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="624" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="624" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A624" t="s">
         <v>85</v>
       </c>
@@ -22844,7 +22847,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="635" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="635" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A635" t="s">
         <v>28</v>
       </c>
@@ -22873,7 +22876,7 @@
         <v>403</v>
       </c>
       <c r="J635">
-        <f>SUM(H635:I635)</f>
+        <f t="shared" ref="J635:J645" si="22">SUM(H635:I635)</f>
         <v>507</v>
       </c>
     </row>
@@ -22906,7 +22909,7 @@
         <v>62</v>
       </c>
       <c r="J636">
-        <f>SUM(H636:I636)</f>
+        <f t="shared" si="22"/>
         <v>86</v>
       </c>
     </row>
@@ -22939,11 +22942,11 @@
         <v>10</v>
       </c>
       <c r="J637">
-        <f>SUM(H637:I637)</f>
+        <f t="shared" si="22"/>
         <v>11</v>
       </c>
     </row>
-    <row r="638" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="638" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A638" t="s">
         <v>12</v>
       </c>
@@ -22972,7 +22975,7 @@
         <v>617</v>
       </c>
       <c r="J638">
-        <f>SUM(H638:I638)</f>
+        <f t="shared" si="22"/>
         <v>747</v>
       </c>
     </row>
@@ -23005,7 +23008,7 @@
         <v>270</v>
       </c>
       <c r="J639">
-        <f>SUM(H639:I639)</f>
+        <f t="shared" si="22"/>
         <v>316</v>
       </c>
     </row>
@@ -23038,11 +23041,11 @@
         <v>53</v>
       </c>
       <c r="J640">
-        <f>SUM(H640:I640)</f>
+        <f t="shared" si="22"/>
         <v>53</v>
       </c>
     </row>
-    <row r="641" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="641" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A641" t="s">
         <v>84</v>
       </c>
@@ -23071,7 +23074,7 @@
         <v>253</v>
       </c>
       <c r="J641">
-        <f>SUM(H641:I641)</f>
+        <f t="shared" si="22"/>
         <v>310</v>
       </c>
     </row>
@@ -23104,11 +23107,11 @@
         <v>105</v>
       </c>
       <c r="J642">
-        <f>SUM(H642:I642)</f>
+        <f t="shared" si="22"/>
         <v>116</v>
       </c>
     </row>
-    <row r="643" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="643" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A643" t="s">
         <v>63</v>
       </c>
@@ -23137,11 +23140,11 @@
         <v>37</v>
       </c>
       <c r="J643">
-        <f>SUM(H643:I643)</f>
+        <f t="shared" si="22"/>
         <v>41</v>
       </c>
     </row>
-    <row r="644" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="644" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A644" t="s">
         <v>55</v>
       </c>
@@ -23170,7 +23173,7 @@
         <v>208</v>
       </c>
       <c r="J644">
-        <f>SUM(H644:I644)</f>
+        <f t="shared" si="22"/>
         <v>267</v>
       </c>
     </row>
@@ -23203,7 +23206,7 @@
         <v>1</v>
       </c>
       <c r="J645">
-        <f>SUM(H645:I645)</f>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
     </row>
@@ -23352,7 +23355,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="651" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="651" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A651" t="s">
         <v>37</v>
       </c>
@@ -23537,7 +23540,7 @@
         <v>85</v>
       </c>
       <c r="J656">
-        <f>SUM(H656:I656)</f>
+        <f t="shared" ref="J656:J664" si="23">SUM(H656:I656)</f>
         <v>103</v>
       </c>
     </row>
@@ -23570,11 +23573,11 @@
         <v>0</v>
       </c>
       <c r="J657">
-        <f>SUM(H657:I657)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
     </row>
-    <row r="658" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="658" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A658" t="s">
         <v>20</v>
       </c>
@@ -23603,7 +23606,7 @@
         <v>78</v>
       </c>
       <c r="J658">
-        <f>SUM(H658:I658)</f>
+        <f t="shared" si="23"/>
         <v>87</v>
       </c>
     </row>
@@ -23636,11 +23639,11 @@
         <v>71</v>
       </c>
       <c r="J659">
-        <f>SUM(H659:I659)</f>
+        <f t="shared" si="23"/>
         <v>72</v>
       </c>
     </row>
-    <row r="660" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="660" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A660" t="s">
         <v>11</v>
       </c>
@@ -23669,7 +23672,7 @@
         <v>59</v>
       </c>
       <c r="J660">
-        <f>SUM(H660:I660)</f>
+        <f t="shared" si="23"/>
         <v>69</v>
       </c>
     </row>
@@ -23702,11 +23705,11 @@
         <v>219</v>
       </c>
       <c r="J661">
-        <f>SUM(H661:I661)</f>
+        <f t="shared" si="23"/>
         <v>237</v>
       </c>
     </row>
-    <row r="662" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="662" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A662" t="s">
         <v>94</v>
       </c>
@@ -23735,11 +23738,11 @@
         <v>52</v>
       </c>
       <c r="J662">
-        <f>SUM(H662:I662)</f>
+        <f t="shared" si="23"/>
         <v>65</v>
       </c>
     </row>
-    <row r="663" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="663" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A663" t="s">
         <v>93</v>
       </c>
@@ -23768,7 +23771,7 @@
         <v>381</v>
       </c>
       <c r="J663">
-        <f>SUM(H663:I663)</f>
+        <f t="shared" si="23"/>
         <v>445</v>
       </c>
     </row>
@@ -23801,7 +23804,7 @@
         <v>0</v>
       </c>
       <c r="J664">
-        <f>SUM(H664:I664)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -23966,7 +23969,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="670" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="670" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A670" t="s">
         <v>7</v>
       </c>
@@ -24003,7 +24006,7 @@
   <autoFilter ref="A1:L670" xr:uid="{2E35D7B2-1B58-4F18-8F20-3FD4FD359FB7}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Kiekenstraat 6, Leuven"/>
+        <filter val="na"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:L670">

</xml_diff>